<commit_message>
add rows for new photos
</commit_message>
<xml_diff>
--- a/labels/phenotype_labels.xlsx
+++ b/labels/phenotype_labels.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavlina/Documents/Helsinki/2nd_Semester/DS_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavlina/Documents/Helsinki/2nd_Semester/DS_project/repo/labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9898E88A-5A52-DA42-AF33-09935BD962C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8518C6B7-2BD4-A248-97E4-7BB42D520893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-13000" yWindow="-28300" windowWidth="22800" windowHeight="28300" xr2:uid="{863811EF-36C7-6E41-B14D-36C7835FD2B1}"/>
   </bookViews>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">birch_labels_final!$A$1:$H$401</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="701">
   <si>
     <t>filename</t>
   </si>
@@ -1952,6 +1965,180 @@
   </si>
   <si>
     <t>IMG_9999 2.jpeg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_1.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_2.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_3.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_4.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_5.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_6.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_7.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_8.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_9.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_10.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_11.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_12.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_13.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_14.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_15.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_16.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_17.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_18.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_19.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_20.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_21.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_22.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_23.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_24.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_25.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_26.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_27.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_28.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_29.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_30.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_31.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_32.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_33.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_34.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_35.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_36.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_37.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_38.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_39.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_40.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_41.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_42.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_43.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_44.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_45.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_46.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_47.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_48.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_49.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_50.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_51.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_52.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_53.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_54.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_55.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_56.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_57.jpg</t>
+  </si>
+  <si>
+    <t>Sampo_7th_March_58.jpg</t>
   </si>
 </sst>
 </file>
@@ -2795,18 +2982,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491470B8-0343-C542-AE89-86889CF720D3}">
-  <dimension ref="A1:H636"/>
+  <dimension ref="A1:H694"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -17411,6 +17598,296 @@
     <row r="636" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A636" t="s">
         <v>642</v>
+      </c>
+    </row>
+    <row r="637" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A637" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="638" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A638" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="639" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A639" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="640" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A640" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="641" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A641" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="642" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A642" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="643" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A643" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="644" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A644" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="645" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A645" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="646" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A646" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="647" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A647" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="648" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A648" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="649" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A649" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="650" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A650" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="651" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A651" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="652" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A652" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="653" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A653" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="654" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A654" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="655" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A655" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="656" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A656" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="657" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A657" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="658" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A658" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="659" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A659" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="660" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A660" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="661" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A661" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="662" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A662" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="663" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A663" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="664" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A664" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="665" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A665" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="666" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A666" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="667" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A667" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="668" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A668" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="669" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A669" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="670" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A670" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="671" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A671" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="672" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A672" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="673" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A673" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="674" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A674" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="675" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A675" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="676" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A676" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="677" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A677" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="678" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A678" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="679" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A679" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="680" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A680" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="681" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A681" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="682" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A682" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="683" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A683" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="684" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A684" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="685" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A685" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="686" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A686" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="687" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A687" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="688" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A688" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="689" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A689" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="690" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A690" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="691" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A691" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="692" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A692" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="693" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A693" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="694" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A694" t="s">
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>